<commit_message>
feat: add solution using Reflection API
</commit_message>
<xml_diff>
--- a/src/main/resources/test_table.xlsx
+++ b/src/main/resources/test_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dima/IdeaProjects/java-exel-converter/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880D5DC7-7A2E-8348-A007-DFE275451357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8184268F-B0A4-8F42-94FD-9B8D4AF9A893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="160">
   <si>
     <t>Individual</t>
   </si>
@@ -483,6 +483,24 @@
   </si>
   <si>
     <t>Class Name</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>hasChildren</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>accountHolder</t>
+  </si>
+  <si>
+    <t>457432</t>
   </si>
 </sst>
 </file>
@@ -493,7 +511,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\.m"/>
     <numFmt numFmtId="165" formatCode="yyyy\.mm"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -546,8 +564,23 @@
       <color theme="1"/>
       <name val="&quot;Liberation Sans&quot;"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -587,25 +620,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor rgb="FFDDE8CB"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FFFFA6A6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FFFFDBB6"/>
       </patternFill>
     </fill>
   </fills>
@@ -651,7 +666,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -675,9 +690,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -713,33 +725,23 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -958,489 +960,487 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:19" ht="15.75" customHeight="1">
+      <c r="A1" s="23"/>
+      <c r="D1" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="O1" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="22" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" customHeight="1">
+      <c r="A2" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1"/>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="4">
-        <v>457532</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" s="6">
-        <v>30</v>
-      </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" ht="15.75" customHeight="1">
+    </row>
+    <row r="3" spans="1:19" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="6" t="b">
+      <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="I3" s="6">
-        <v>32</v>
-      </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" s="8" t="s">
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3" s="6">
+        <v>30</v>
+      </c>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="Q3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="S3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="O3" s="7"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:17" ht="15.75" customHeight="1">
+    </row>
+    <row r="4" spans="1:19" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4" s="6">
         <v>32</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="6">
-        <v>35</v>
-      </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="N4" s="8" t="s">
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="Q4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="S4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="7"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:17" ht="15.75" customHeight="1">
+    </row>
+    <row r="5" spans="1:19" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="2">
-        <v>4</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="6" t="b">
+      <c r="D5" s="2">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="I5" s="10">
-        <v>18</v>
-      </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="N5" s="8" t="s">
+      <c r="L5" s="6">
+        <v>35</v>
+      </c>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="Q5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="O5" s="7"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="1:17" ht="15.75" customHeight="1">
+    </row>
+    <row r="6" spans="1:19" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="2">
+      <c r="D6" s="2">
+        <v>4</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" s="9">
+        <v>18</v>
+      </c>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="Q6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="S6" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="4">
+      <c r="F7" s="24">
         <v>5495493</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="J7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="6" t="b">
+      <c r="K7" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="I6" s="6">
+      <c r="L7" s="6">
         <v>43</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="7" t="s">
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="Q7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="R7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="S7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="O6" s="7"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2">
-        <v>6</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="11">
-        <v>621123456</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="N7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="O7" s="7"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="1"/>
-    </row>
-    <row r="8" spans="1:17" ht="15.75" customHeight="1">
+    </row>
+    <row r="8" spans="1:19" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="2">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="11">
-        <v>621654321</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="D8" s="2">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="26">
+        <v>621123456</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>47</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" s="8" t="s">
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="N8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="O8" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="R8" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="7"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="1"/>
-    </row>
-    <row r="9" spans="1:17" ht="15.75" customHeight="1">
+    </row>
+    <row r="9" spans="1:19" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="2">
-        <v>8</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="11">
-        <v>621369258</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="D9" s="2">
+        <v>7</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="26">
+        <v>621654321</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M9" s="7" t="s">
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="N9" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="R9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="N9" s="8" t="s">
+      <c r="S9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="O9" s="7"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="1"/>
-    </row>
-    <row r="10" spans="1:17" ht="15.75" customHeight="1">
+    </row>
+    <row r="10" spans="1:19" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="2">
-        <v>9</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="11">
-        <v>621147852</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="D10" s="2">
+        <v>8</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="26">
+        <v>621369258</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="N10" s="8" t="s">
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="N10" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="O10" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="R10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="S10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="O10" s="7"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="1:17" ht="15.75" customHeight="1">
+    </row>
+    <row r="11" spans="1:19" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="2">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="11">
-        <v>621789456</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="D11" s="2">
+        <v>9</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="26">
+        <v>621147852</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>60</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="12" t="s">
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="N11" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="O11" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="R11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="S11" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" s="21" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
+        <v>10</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="26">
+        <v>621789456</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="O12" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="L11" s="7" t="s">
+      <c r="P12"/>
+      <c r="Q12" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="M11" s="7" t="s">
+      <c r="R12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="N11" s="8" t="s">
+      <c r="S12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="O11" s="7"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="1:17" s="31" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A12" s="24"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="27"/>
-    </row>
-    <row r="13" spans="1:17" ht="15.75" customHeight="1">
+    </row>
+    <row r="13" spans="1:19" ht="15.75" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1459,7 +1459,7 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="1:17" ht="15.75" customHeight="1">
+    <row r="14" spans="1:19" ht="15.75" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1478,7 +1478,7 @@
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="15" spans="1:17" ht="15.75" customHeight="1">
+    <row r="15" spans="1:19" ht="15.75" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1514,858 +1514,858 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="12" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A3" s="15">
+      <c r="A3" s="14">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="15">
         <v>1</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="16">
         <v>45108</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="14">
         <v>500946941</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="K3" s="16" t="b">
+      <c r="K3" s="15" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A4" s="15">
+      <c r="A4" s="14">
         <v>2</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="15">
         <v>2</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="16">
         <v>45108</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="14">
         <v>500946941</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="K4" s="16" t="b">
+      <c r="K4" s="15" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A5" s="15">
+      <c r="A5" s="14">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="15">
         <v>3</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="16">
         <v>45108</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="14">
         <v>500946941</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="18">
         <v>244166</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="J5" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="K5" s="16" t="b">
+      <c r="K5" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A6" s="15">
+      <c r="A6" s="14">
         <v>4</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="15">
         <v>4</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <v>45108</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="14">
         <v>500946941</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="J6" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="K6" s="16" t="b">
+      <c r="K6" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A7" s="15">
+      <c r="A7" s="14">
         <v>5</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="15">
         <v>1</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="16">
         <v>45108</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="14">
         <v>500946941</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="18">
         <v>9011</v>
       </c>
-      <c r="J7" s="18" t="s">
+      <c r="J7" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="K7" s="16" t="b">
+      <c r="K7" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A8" s="15">
+      <c r="A8" s="14">
         <v>6</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="15">
         <v>2</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="16">
         <v>45108</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="14">
         <v>500946941</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="J8" s="18" t="s">
+      <c r="J8" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="16" t="b">
+      <c r="K8" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A9" s="15">
+      <c r="A9" s="14">
         <v>7</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="15">
         <v>3</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="16">
         <v>45108</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="14">
         <v>500946941</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="J9" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="K9" s="16" t="b">
+      <c r="K9" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A10" s="15">
+      <c r="A10" s="14">
         <v>8</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="15">
         <v>4</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="16">
         <v>45108</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="14">
         <v>500946941</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="18">
         <v>86290</v>
       </c>
-      <c r="J10" s="18" t="s">
+      <c r="J10" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="K10" s="16" t="b">
+      <c r="K10" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A11" s="15">
+      <c r="A11" s="14">
         <v>9</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="15">
         <v>4</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="16">
         <v>45108</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="14">
         <v>500946941</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="I11" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="J11" s="18" t="s">
+      <c r="J11" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="K11" s="16" t="b">
+      <c r="K11" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A12" s="15">
+      <c r="A12" s="14">
         <v>10</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="15">
         <v>5</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="16">
         <v>45108</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="14">
         <v>500946941</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="I12" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="J12" s="18" t="s">
+      <c r="J12" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="K12" s="16" t="b">
+      <c r="K12" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A13" s="15">
+      <c r="A13" s="14">
         <v>11</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="15">
         <v>6</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="16">
         <v>45108</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="14">
         <v>500946941</v>
       </c>
-      <c r="I13" s="15" t="s">
+      <c r="I13" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="J13" s="18" t="s">
+      <c r="J13" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="K13" s="16" t="b">
+      <c r="K13" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A14" s="15">
+      <c r="A14" s="14">
         <v>12</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="15">
         <v>4</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="16">
         <v>45108</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="14">
         <v>500946941</v>
       </c>
-      <c r="I14" s="15" t="s">
+      <c r="I14" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="J14" s="18" t="s">
+      <c r="J14" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="K14" s="16" t="b">
+      <c r="K14" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A15" s="15">
+      <c r="A15" s="14">
         <v>13</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="15">
         <v>3</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="16">
         <v>45108</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="G15" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="14">
         <v>500946941</v>
       </c>
-      <c r="I15" s="15" t="s">
+      <c r="I15" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="J15" s="18" t="s">
+      <c r="J15" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="K15" s="16" t="b">
+      <c r="K15" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A16" s="15">
+      <c r="A16" s="14">
         <v>14</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="15">
         <v>2</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="16">
         <v>45108</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="G16" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="H16" s="15">
+      <c r="H16" s="14">
         <v>500946941</v>
       </c>
-      <c r="I16" s="15" t="s">
+      <c r="I16" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="J16" s="18" t="s">
+      <c r="J16" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="K16" s="16" t="b">
+      <c r="K16" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A17" s="15">
+      <c r="A17" s="14">
         <v>15</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="15">
         <v>5</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="16">
         <v>45108</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="G17" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="H17" s="15">
+      <c r="H17" s="14">
         <v>500946941</v>
       </c>
-      <c r="I17" s="15" t="s">
+      <c r="I17" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="J17" s="18" t="s">
+      <c r="J17" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="K17" s="16" t="b">
+      <c r="K17" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A18" s="15">
+      <c r="A18" s="14">
         <v>16</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="15">
         <v>6</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="16">
         <v>45108</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="G18" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="H18" s="15">
+      <c r="H18" s="14">
         <v>500946941</v>
       </c>
-      <c r="I18" s="15" t="s">
+      <c r="I18" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="J18" s="16" t="s">
+      <c r="J18" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="K18" s="16" t="b">
+      <c r="K18" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A19" s="15">
+      <c r="A19" s="14">
         <v>17</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="15">
         <v>8</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="16">
         <v>45108</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="F19" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H19" s="14">
         <v>500946941</v>
       </c>
-      <c r="I19" s="20" t="s">
+      <c r="I19" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="J19" s="16" t="s">
+      <c r="J19" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="K19" s="16" t="b">
+      <c r="K19" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A20" s="15">
+      <c r="A20" s="14">
         <v>18</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C20" s="15">
         <v>9</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="16">
         <v>45108</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="H20" s="15">
+      <c r="H20" s="14">
         <v>500946941</v>
       </c>
-      <c r="I20" s="15" t="s">
+      <c r="I20" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="J20" s="16" t="s">
+      <c r="J20" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="K20" s="16" t="b">
+      <c r="K20" s="15" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A21" s="15">
+      <c r="A21" s="14">
         <v>19</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C21" s="15">
         <v>10</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="16">
         <v>45108</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21" s="14">
         <v>500946941</v>
       </c>
-      <c r="I21" s="20" t="s">
+      <c r="I21" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="J21" s="16" t="s">
+      <c r="J21" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="K21" s="16" t="b">
+      <c r="K21" s="15" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A22" s="15">
+      <c r="A22" s="14">
         <v>20</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="C22" s="16">
+      <c r="C22" s="15">
         <v>3</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="16">
         <v>45108</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="F22" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="G22" s="16" t="s">
+      <c r="G22" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="H22" s="15">
+      <c r="H22" s="14">
         <v>500946941</v>
       </c>
-      <c r="I22" s="15" t="s">
+      <c r="I22" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="J22" s="16" t="s">
+      <c r="J22" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="K22" s="16" t="b">
+      <c r="K22" s="15" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A23" s="15"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A24" s="15"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A25" s="15"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
+      <c r="A25" s="14"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A26" s="15"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A27" s="15"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="15"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A28" s="15"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A29" s="15"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A30" s="15"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
+      <c r="A30" s="14"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
feat: update table file
</commit_message>
<xml_diff>
--- a/src/main/resources/test_table.xlsx
+++ b/src/main/resources/test_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dima/IdeaProjects/java-exel-converter/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8184268F-B0A4-8F42-94FD-9B8D4AF9A893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB7B631-9523-6A41-BAF5-03F2F2AF4B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -962,29 +962,31 @@
   </sheetPr>
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" customHeight="1">
       <c r="A1" s="23"/>
+      <c r="C1" s="22" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="22" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="22" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="22"/>
       <c r="I1" s="22" t="s">
         <v>154</v>
       </c>
@@ -1017,16 +1019,16 @@
       <c r="A2" s="20" t="s">
         <v>153</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -1061,18 +1063,19 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2">
+      <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="E3" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="G3" s="22"/>
       <c r="I3" s="5" t="s">
         <v>17</v>
       </c>
@@ -1101,18 +1104,19 @@
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="2">
+      <c r="C4" s="2">
         <v>2</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="E4" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="G4" s="22"/>
       <c r="I4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1141,18 +1145,19 @@
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="2">
+      <c r="C5" s="2">
         <v>3</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="E5" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="G5" s="22"/>
       <c r="I5" s="5" t="s">
         <v>32</v>
       </c>
@@ -1181,18 +1186,19 @@
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="2">
+      <c r="C6" s="2">
         <v>4</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="E6" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="G6" s="22"/>
       <c r="I6" s="5" t="s">
         <v>39</v>
       </c>
@@ -1221,18 +1227,19 @@
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="2">
+      <c r="C7" s="2">
         <v>5</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="24">
+      <c r="E7" s="24">
         <v>5495493</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="G7" s="22"/>
       <c r="I7" s="5" t="s">
         <v>43</v>
       </c>
@@ -1261,18 +1268,19 @@
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="2">
+      <c r="C8" s="2">
         <v>6</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="26">
+      <c r="E8" s="26">
         <v>621123456</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="F8" s="10" t="s">
         <v>47</v>
       </c>
+      <c r="G8" s="22"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1297,18 +1305,19 @@
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="2">
+      <c r="C9" s="2">
         <v>7</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="26">
+      <c r="E9" s="26">
         <v>621654321</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>53</v>
       </c>
+      <c r="G9" s="22"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1333,18 +1342,19 @@
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="2">
+      <c r="C10" s="2">
         <v>8</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="26">
+      <c r="E10" s="26">
         <v>621369258</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>57</v>
       </c>
+      <c r="G10" s="22"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1369,18 +1379,19 @@
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="2">
+      <c r="C11" s="2">
         <v>9</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="26">
+      <c r="E11" s="26">
         <v>621147852</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>60</v>
       </c>
+      <c r="G11" s="22"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1405,18 +1416,19 @@
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="2">
+      <c r="C12" s="2">
         <v>10</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="26">
+      <c r="E12" s="26">
         <v>621789456</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>63</v>
       </c>
+      <c r="G12" s="22"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>

</xml_diff>